<commit_message>
Attempts at GUI development
</commit_message>
<xml_diff>
--- a/Questionnaire/Questionnaire_Questions_master.xlsx
+++ b/Questionnaire/Questionnaire_Questions_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgomezd1\repos\RepoRepli\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C9E6C5B-81E3-42DE-9CB4-D71438F69F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA812517-5BE8-4685-8396-05EF0BCC8C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26C12347-018D-44EE-A7C4-D1B81FA78D51}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26C12347-018D-44EE-A7C4-D1B81FA78D51}"/>
   </bookViews>
   <sheets>
     <sheet name="Fitting" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="29">
   <si>
     <t>Question_ID</t>
   </si>
@@ -69,12 +69,6 @@
     <t>Not_Equivalent_or_Applicable</t>
   </si>
   <si>
-    <t>Are the data pre-processing computations (e.g., normalization, imputation) equivalent?</t>
-  </si>
-  <si>
-    <t>Yes. The method of preprocessing the data is the same and is carried out in a fully equivalent computational environment.</t>
-  </si>
-  <si>
     <t>Somewhat. The method for preprocessing the data includes more or fewer stepts, or the preprocessing environment is different in a way that may materially affect the results.</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>Almost. The fitting metric is computationally a bit different, but should provide equivalent results - or the computation of the metric isn't the same but shouldn't materially affect the results.</t>
   </si>
   <si>
-    <t>Almost. The method of preprocessing the data is different but should provide equivalent results - or the preprocessing computations are different but shouldn't materially affect the results.</t>
-  </si>
-  <si>
     <t>Somewhat. The computation of the fitting metric is different enough that it may materially affect the results. (e.g., it's computed over a differently sized set of samples)</t>
   </si>
   <si>
@@ -115,6 +106,28 @@
   </si>
   <si>
     <t>Lorem Ipsum</t>
+  </si>
+  <si>
+    <t>Is the algorithm used in your study equivalent to that used in the base study?</t>
+  </si>
+  <si>
+    <t>Yes. The same algorithm is used within an equivalent computational environment.</t>
+  </si>
+  <si>
+    <t>Almost. The algorithm is designed to address the same task as in the base study in a similar fashion, nad the difference shouldn't materially affect the results.</t>
+  </si>
+  <si>
+    <t>Are the data pre-processing computations 
+(e.g., normalization, imputation) equivalent?</t>
+  </si>
+  <si>
+    <t>Yes. The method of preprocessing the data is the same and is
+carried out in a fully equivalent computational environment.</t>
+  </si>
+  <si>
+    <t>Almost. The method of preprocessing the data is different 
+but should provide equivalent results - or the preprocessing 
+computations are different but shouldn't materially affect the results.</t>
   </si>
 </sst>
 </file>
@@ -476,7 +489,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,19 +530,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -540,19 +553,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -563,19 +576,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -583,22 +596,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -609,19 +622,19 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -632,19 +645,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -655,19 +668,19 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -678,19 +691,19 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -701,19 +714,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -724,19 +737,19 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -747,19 +760,19 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -770,19 +783,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -793,19 +806,19 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -816,19 +829,19 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -839,19 +852,19 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -862,19 +875,19 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -885,19 +898,19 @@
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -908,19 +921,19 @@
         <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -931,19 +944,19 @@
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -954,19 +967,19 @@
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -977,19 +990,19 @@
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1311,19 +1324,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1334,19 +1347,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1357,19 +1370,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1380,19 +1393,19 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1403,19 +1416,19 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1426,19 +1439,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1449,19 +1462,19 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1472,19 +1485,19 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1495,19 +1508,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1518,19 +1531,19 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1541,19 +1554,19 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1564,19 +1577,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1587,19 +1600,19 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1610,19 +1623,19 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1633,19 +1646,19 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1656,19 +1669,19 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1679,19 +1692,19 @@
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1702,19 +1715,19 @@
         <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1725,19 +1738,19 @@
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1748,19 +1761,19 @@
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1771,19 +1784,19 @@
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -2059,6 +2072,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B95A8CAD8C29554F9E0351C467B0D6FD" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="1b39f6b3157a2808afb706e2abc1a757">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xmlns:ns4="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b35085bbad307f65ab8a7111ba96ce01" ns3:_="" ns4:_="">
     <xsd:import namespace="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
@@ -2305,24 +2335,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1904384E-797A-433F-B14D-F7DBECBCF5A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
+    <ds:schemaRef ds:uri="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23A7755D-48E6-4A04-985B-2FF9CD4824DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8304BA-87CC-4068-8193-05A133AC1626}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2339,29 +2377,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23A7755D-48E6-4A04-985B-2FF9CD4824DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1904384E-797A-433F-B14D-F7DBECBCF5A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
-    <ds:schemaRef ds:uri="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated to generate questions from excel
</commit_message>
<xml_diff>
--- a/Questionnaire/Questionnaire_Questions_master.xlsx
+++ b/Questionnaire/Questionnaire_Questions_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgomezd1\repos\RepoRepli\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA812517-5BE8-4685-8396-05EF0BCC8C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64237A17-DC9D-472E-BF52-12F18951BA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26C12347-018D-44EE-A7C4-D1B81FA78D51}"/>
   </bookViews>
@@ -121,13 +121,10 @@
 (e.g., normalization, imputation) equivalent?</t>
   </si>
   <si>
-    <t>Yes. The method of preprocessing the data is the same and is
-carried out in a fully equivalent computational environment.</t>
-  </si>
-  <si>
-    <t>Almost. The method of preprocessing the data is different 
-but should provide equivalent results - or the preprocessing 
-computations are different but shouldn't materially affect the results.</t>
+    <t>Yes. The method of preprocessing the data is the same and is carried out in a fully equivalent computational environment.</t>
+  </si>
+  <si>
+    <t>Almost. The method of preprocessing the data is different but should provide equivalent results - or the preprocessing computations are different but shouldn't materially affect the results.</t>
   </si>
 </sst>
 </file>
@@ -489,7 +486,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2072,23 +2069,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B95A8CAD8C29554F9E0351C467B0D6FD" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="1b39f6b3157a2808afb706e2abc1a757">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xmlns:ns4="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b35085bbad307f65ab8a7111ba96ce01" ns3:_="" ns4:_="">
     <xsd:import namespace="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
@@ -2335,32 +2315,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1904384E-797A-433F-B14D-F7DBECBCF5A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
-    <ds:schemaRef ds:uri="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23A7755D-48E6-4A04-985B-2FF9CD4824DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8304BA-87CC-4068-8193-05A133AC1626}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2377,4 +2349,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23A7755D-48E6-4A04-985B-2FF9CD4824DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1904384E-797A-433F-B14D-F7DBECBCF5A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
+    <ds:schemaRef ds:uri="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to questionnaire in progress
</commit_message>
<xml_diff>
--- a/Questionnaire/Questionnaire_Questions_master.xlsx
+++ b/Questionnaire/Questionnaire_Questions_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgomezd1\repos\RepoRepli\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64237A17-DC9D-472E-BF52-12F18951BA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B913B-0C69-42FA-BA0B-53A12BDF1E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26C12347-018D-44EE-A7C4-D1B81FA78D51}"/>
+    <workbookView xWindow="-38520" yWindow="-2850" windowWidth="38640" windowHeight="21120" xr2:uid="{26C12347-018D-44EE-A7C4-D1B81FA78D51}"/>
   </bookViews>
   <sheets>
     <sheet name="Fitting" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="51">
   <si>
     <t>Question_ID</t>
   </si>
@@ -69,62 +69,127 @@
     <t>Not_Equivalent_or_Applicable</t>
   </si>
   <si>
-    <t>Somewhat. The method for preprocessing the data includes more or fewer stepts, or the preprocessing environment is different in a way that may materially affect the results.</t>
-  </si>
-  <si>
-    <t>Not equivalent or applicable. The preprocessing is substantially different, or the preprocessing environment will certainly materially affect the results (e.g., using a float8 variables because of limitations)</t>
-  </si>
-  <si>
-    <t>Are the fitting metric computations (e.g., the loss function) equivalent?</t>
-  </si>
-  <si>
-    <t>Yes. The fitting metric is the same and are calculation is carried out in a fully equivalent computational environment.</t>
-  </si>
-  <si>
-    <t>Almost. The fitting metric is computationally a bit different, but should provide equivalent results - or the computation of the metric isn't the same but shouldn't materially affect the results.</t>
-  </si>
-  <si>
-    <t>Somewhat. The computation of the fitting metric is different enough that it may materially affect the results. (e.g., it's computed over a differently sized set of samples)</t>
-  </si>
-  <si>
-    <t>Not equivalent or applicable. The fitting metric is substantially different, or the computational environment will certainly materially affect the results</t>
-  </si>
-  <si>
-    <t>Are the model fitting computations (e.g., the implementation and its hyperparameters) equivalent?</t>
-  </si>
-  <si>
-    <t>Yes. The computations for fitting the model are carried out in a fully equivalent way in a fully equivalent computational environment.</t>
-  </si>
-  <si>
-    <t>Almost. The computations for fitting the model are similar but may vary in their implementations, or the computation of the model is different in a way that doesn't materially affect the results.</t>
-  </si>
-  <si>
-    <t>Somewhat. The fitting computations are different enough that they may materially affect the results (e.g., the method for solving model parameters)</t>
-  </si>
-  <si>
-    <t>Not equivalent or applicable. The model computation is different in a way that will certainly materially affect the results (e.g., important hyper-parameters cannot have the same value as in the base study)</t>
-  </si>
-  <si>
     <t>Lorem Ipsum</t>
   </si>
   <si>
-    <t>Is the algorithm used in your study equivalent to that used in the base study?</t>
-  </si>
-  <si>
-    <t>Yes. The same algorithm is used within an equivalent computational environment.</t>
-  </si>
-  <si>
-    <t>Almost. The algorithm is designed to address the same task as in the base study in a similar fashion, nad the difference shouldn't materially affect the results.</t>
-  </si>
-  <si>
-    <t>Are the data pre-processing computations 
-(e.g., normalization, imputation) equivalent?</t>
-  </si>
-  <si>
-    <t>Yes. The method of preprocessing the data is the same and is carried out in a fully equivalent computational environment.</t>
-  </si>
-  <si>
-    <t>Almost. The method of preprocessing the data is different but should provide equivalent results - or the preprocessing computations are different but shouldn't materially affect the results.</t>
+    <t>Is the computational processing of the fitting dataset equivalent?</t>
+  </si>
+  <si>
+    <t>Are the predictors selected for model fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Is the method used to select the predictors used for fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Is the definition of the target event equivalent?</t>
+  </si>
+  <si>
+    <t>Are the preprocessing steps applied to the predictors before fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Are the preprocessing steps applied to the target variable(s) before fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Is the dataset size used for model fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Is the method for partitioning the dataset into folds for use in fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Is the way the evaluation metrics are calculated or implemented for model fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Is the set of metrics chosen for use in model fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Is the use of the chosen metrics within fitting optimization equivalent?</t>
+  </si>
+  <si>
+    <t>Are the observed va;ues of the metrics chosen for fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Is the computational implementation of the algorithm equivalent?</t>
+  </si>
+  <si>
+    <t>Is the range of hyperparameters explored equivalent?</t>
+  </si>
+  <si>
+    <t>Is the stragegy used to search the hyperparameter space equivalent?</t>
+  </si>
+  <si>
+    <t>Are the best hyperparameters discovered during the search equivalent?</t>
+  </si>
+  <si>
+    <t>Are the learnable parameters observed after fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Somewhat. The method for preprocessing the data includes moderate differences in implementation, leading to materially different outcomes</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. The preprocessing is inculdes substantial differences or completely different computational approaches are used</t>
+  </si>
+  <si>
+    <t>Yes. The method of preprocessing the data is the same and is carried out in a fully equivalent computational environment</t>
+  </si>
+  <si>
+    <t>Yes. The same set of predictors or  a fully equivalent set of predictors is used</t>
+  </si>
+  <si>
+    <t>Almost. The method includes minor variations in implementation, resulting in approximately similar outcomes</t>
+  </si>
+  <si>
+    <t>Almost. There is a slight variation in the set of predictors used, but approximately similar outcomes are expected.</t>
+  </si>
+  <si>
+    <t>Somewhat. The predictor set exhibits moderate differences and a material effect on the outcomes is expected</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable.</t>
+  </si>
+  <si>
+    <t>Yes.</t>
+  </si>
+  <si>
+    <t>Almost.</t>
+  </si>
+  <si>
+    <t>Somewhat.</t>
+  </si>
+  <si>
+    <t>Yes. The same strategy or a fully equivalent stratefy for selecting the predictors is used</t>
+  </si>
+  <si>
+    <t>Almost. There is slight variation in the strategy used to select the predictors, but approximately similar outcomes are expected</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. The strategy used to select predictors is substantially different</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. A substantially different sets of predictors is utilized</t>
+  </si>
+  <si>
+    <t>Yes. The target event definitions are identical or fully equivalent</t>
+  </si>
+  <si>
+    <t>Almost. There is slight variation in the target event definitions, but approximately similar outcomes are expected</t>
+  </si>
+  <si>
+    <t>Somewhat. There are moderate differences in target event definitions, and a material effect on the outcomes is expected</t>
+  </si>
+  <si>
+    <t>Somewhat. The strategy used to select the predictors exhibits moderate differences and a material difference in the outcomes is expected</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. The target definition is substantially different.</t>
+  </si>
+  <si>
+    <t>Yes.  The same or  fully equivalent set of preprocessing steps is used</t>
+  </si>
+  <si>
+    <t>Almost.  There is a slight variation in the preprocessing steps being used, but approximately similar outcomes are expected</t>
+  </si>
+  <si>
+    <t>Somewhat.There are moderate differences in the data preprocessing steps, and a material effect on the outcomes is expected</t>
   </si>
 </sst>
 </file>
@@ -486,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,19 +592,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -547,22 +612,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -570,22 +635,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -593,22 +658,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -616,22 +681,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -639,22 +704,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -665,19 +730,19 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -685,22 +750,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -708,22 +773,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -731,22 +796,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -757,19 +822,19 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -777,22 +842,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -800,22 +865,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -823,22 +888,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -849,19 +914,19 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -869,22 +934,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -892,115 +957,51 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
@@ -1278,7 +1279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E887A27C-ABA9-4134-A972-BB4D9C343E58}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
@@ -1321,19 +1322,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1344,19 +1345,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1367,19 +1368,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1390,19 +1391,19 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1413,19 +1414,19 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1436,19 +1437,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1459,19 +1460,19 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1482,19 +1483,19 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1505,19 +1506,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1528,19 +1529,19 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1551,19 +1552,19 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1574,19 +1575,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1597,19 +1598,19 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1620,19 +1621,19 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1643,19 +1644,19 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1666,19 +1667,19 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1689,19 +1690,19 @@
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1712,19 +1713,19 @@
         <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1735,19 +1736,19 @@
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1758,19 +1759,19 @@
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1781,19 +1782,19 @@
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -2069,6 +2070,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B95A8CAD8C29554F9E0351C467B0D6FD" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="1b39f6b3157a2808afb706e2abc1a757">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xmlns:ns4="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b35085bbad307f65ab8a7111ba96ce01" ns3:_="" ns4:_="">
     <xsd:import namespace="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
@@ -2315,24 +2333,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1904384E-797A-433F-B14D-F7DBECBCF5A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
+    <ds:schemaRef ds:uri="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23A7755D-48E6-4A04-985B-2FF9CD4824DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8304BA-87CC-4068-8193-05A133AC1626}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2349,29 +2375,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23A7755D-48E6-4A04-985B-2FF9CD4824DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1904384E-797A-433F-B14D-F7DBECBCF5A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
-    <ds:schemaRef ds:uri="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated question list and some answers
</commit_message>
<xml_diff>
--- a/Questionnaire/Questionnaire_Questions_master.xlsx
+++ b/Questionnaire/Questionnaire_Questions_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgomezd1\repos\RepoRepli\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B913B-0C69-42FA-BA0B-53A12BDF1E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F888CC-9A84-4A1A-B13E-FD0ACD4B7B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2850" windowWidth="38640" windowHeight="21120" xr2:uid="{26C12347-018D-44EE-A7C4-D1B81FA78D51}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="14796" windowHeight="12336" activeTab="1" xr2:uid="{26C12347-018D-44EE-A7C4-D1B81FA78D51}"/>
   </bookViews>
   <sheets>
     <sheet name="Fitting" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="83">
   <si>
     <t>Question_ID</t>
   </si>
@@ -96,18 +96,12 @@
     <t>Is the method for partitioning the dataset into folds for use in fitting equivalent?</t>
   </si>
   <si>
-    <t>Is the way the evaluation metrics are calculated or implemented for model fitting equivalent?</t>
-  </si>
-  <si>
     <t>Is the set of metrics chosen for use in model fitting equivalent?</t>
   </si>
   <si>
     <t>Is the use of the chosen metrics within fitting optimization equivalent?</t>
   </si>
   <si>
-    <t>Are the observed va;ues of the metrics chosen for fitting equivalent?</t>
-  </si>
-  <si>
     <t>Is the computational implementation of the algorithm equivalent?</t>
   </si>
   <si>
@@ -135,12 +129,6 @@
     <t>Yes. The same set of predictors or  a fully equivalent set of predictors is used</t>
   </si>
   <si>
-    <t>Almost. The method includes minor variations in implementation, resulting in approximately similar outcomes</t>
-  </si>
-  <si>
-    <t>Almost. There is a slight variation in the set of predictors used, but approximately similar outcomes are expected.</t>
-  </si>
-  <si>
     <t>Somewhat. The predictor set exhibits moderate differences and a material effect on the outcomes is expected</t>
   </si>
   <si>
@@ -159,9 +147,6 @@
     <t>Yes. The same strategy or a fully equivalent stratefy for selecting the predictors is used</t>
   </si>
   <si>
-    <t>Almost. There is slight variation in the strategy used to select the predictors, but approximately similar outcomes are expected</t>
-  </si>
-  <si>
     <t>Not equivalent or applicable. The strategy used to select predictors is substantially different</t>
   </si>
   <si>
@@ -171,9 +156,6 @@
     <t>Yes. The target event definitions are identical or fully equivalent</t>
   </si>
   <si>
-    <t>Almost. There is slight variation in the target event definitions, but approximately similar outcomes are expected</t>
-  </si>
-  <si>
     <t>Somewhat. There are moderate differences in target event definitions, and a material effect on the outcomes is expected</t>
   </si>
   <si>
@@ -186,10 +168,124 @@
     <t>Yes.  The same or  fully equivalent set of preprocessing steps is used</t>
   </si>
   <si>
-    <t>Almost.  There is a slight variation in the preprocessing steps being used, but approximately similar outcomes are expected</t>
-  </si>
-  <si>
-    <t>Somewhat.There are moderate differences in the data preprocessing steps, and a material effect on the outcomes is expected</t>
+    <t xml:space="preserve">Yes. The same or fully equivalent preprocessing steps are applied to the target variable before fitting </t>
+  </si>
+  <si>
+    <t>Somewhat.There are moderate differences in the predictor preprocessing steps, and a material effect on the outcomes is expected</t>
+  </si>
+  <si>
+    <t>Somewhat. There are moderate differences in the target preprocessing steps, and a material effect on the outcomes is expected</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. The predictor data preprocessing steps are substantially different</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. The target data preprocessing steps are substantially different</t>
+  </si>
+  <si>
+    <t>Yes. The number of samples in the dataset is exactly the same or fully equivalent</t>
+  </si>
+  <si>
+    <t>Almost. The is a slight variation in the number of samples in the dataset, but the reflected distribution is expected to be approximately the same</t>
+  </si>
+  <si>
+    <t>Somewhat. There is a moderate variation in the number of samples in the dataset, and the reflected distribution is expected to be materially affected</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. The number of samples in the dataset and/or the reflected distribution is substantially different</t>
+  </si>
+  <si>
+    <t>Yes. The number of data folds and the method used to create them is exactly the same or fully equivalent</t>
+  </si>
+  <si>
+    <t>Almost. There is a slight variation in the number of data folds and/or the method used to create them, but should result in approximately the same behavior</t>
+  </si>
+  <si>
+    <t>Somewhat. There is a moderate variation in the number of data folds and/or the method used to create them, and a material change in behavior is expected</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. The number of data folds and/or the method used to create them is substantially different</t>
+  </si>
+  <si>
+    <t>Almost. There are minor variations in calculation methods, but the metric values should be similar</t>
+  </si>
+  <si>
+    <t>Somewhat. Moderate varitions in the calculation values can result in material differences in metric values</t>
+  </si>
+  <si>
+    <t>Is the way the fitting metrics are calculated and/or implemented equivalent?</t>
+  </si>
+  <si>
+    <t>Yes. Identical or fully equivalent methods are used to calculate the metrics</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. The calculation of the metric values are substantially different</t>
+  </si>
+  <si>
+    <t>Yes. The set of metrics used to fit the model is defined and utilized in the same way, or a fully equivalent way</t>
+  </si>
+  <si>
+    <t>Almost. There is a slight variation in the set of metrics used to fit the model or how they are utilized, but  similar outcomes are expected</t>
+  </si>
+  <si>
+    <t>Almost. There is a slight variation in the preprocessing steps applied to the target variable, but  similar outcomes are expected</t>
+  </si>
+  <si>
+    <t>Almost.  There is a slight variation in the preprocessing steps being used on the predictors, but similar outcomes are expected</t>
+  </si>
+  <si>
+    <t>Almost. There is a slight variation in the target event definitions, but similar outcomes are expected</t>
+  </si>
+  <si>
+    <t>Almost. There is slight variation in the strategy used to select the predictors, but similar outcomes are expected</t>
+  </si>
+  <si>
+    <t>Almost. There is a slight variation in the set of predictors used, but similar outcomes are expected.</t>
+  </si>
+  <si>
+    <t>Almost. The method includes minor variations in implementation, resulting in similar outcomes</t>
+  </si>
+  <si>
+    <t>Somewhat. Moderate changes in the set of metrics used to fit the model or how they are utilized are expected to materially affect the outcomes</t>
+  </si>
+  <si>
+    <t>Not equivalent or applicable. The set of metrics used to fit the model or the method of using them are substantially different</t>
+  </si>
+  <si>
+    <t>Is the computational processing of the evaluation dataset equivalent?</t>
+  </si>
+  <si>
+    <t>Are the predictors used with the model equivalent?</t>
+  </si>
+  <si>
+    <t>Are the preprocessing steps applied to the predictors before evaluation equivalent?</t>
+  </si>
+  <si>
+    <t>Are the preprocessing steps applied to the target variable(s) before evaluation equivalent?</t>
+  </si>
+  <si>
+    <t>Are the model fitting and model evaluation datasets equivalent?</t>
+  </si>
+  <si>
+    <t>Is the dataset size used for model evaluation equivalent?</t>
+  </si>
+  <si>
+    <t>Is the method for partitioning the dataset into folds for evaluation equivalent?</t>
+  </si>
+  <si>
+    <t>Is the way the evaluation metrics are calculated and/or implemented equivalent?</t>
+  </si>
+  <si>
+    <t>Is the set of metrics chosen for model evaluation equivalent?</t>
+  </si>
+  <si>
+    <t>Are the observed values of the metrics chosen for fitting equivalent?</t>
+  </si>
+  <si>
+    <t>Are the structural hyperparameters of the model equivalent?</t>
+  </si>
+  <si>
+    <t>Are the learned parameters in the model equivalent?</t>
   </si>
 </sst>
 </file>
@@ -205,12 +301,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -225,12 +327,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -549,9 +654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D014E6-8A50-44C1-91BB-BEA717BB425C}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,16 +700,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -618,16 +723,16 @@
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -641,16 +746,16 @@
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -664,16 +769,16 @@
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -687,16 +792,16 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -710,16 +815,16 @@
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -733,16 +838,16 @@
         <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -756,16 +861,16 @@
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -776,19 +881,19 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -799,19 +904,19 @@
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -822,19 +927,19 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -845,19 +950,19 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -868,19 +973,19 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -891,19 +996,19 @@
         <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -914,19 +1019,19 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -937,19 +1042,19 @@
         <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -960,19 +1065,19 @@
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1277,11 +1382,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E887A27C-ABA9-4134-A972-BB4D9C343E58}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,7 +1427,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -1342,10 +1447,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -1365,10 +1470,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -1391,7 +1496,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -1411,10 +1516,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -1434,10 +1539,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -1460,7 +1565,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -1480,10 +1585,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -1503,10 +1608,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -1526,10 +1631,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
@@ -1552,7 +1657,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
@@ -1575,7 +1680,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>10</v>
@@ -1595,10 +1700,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>
@@ -1618,10 +1723,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>10</v>
@@ -1637,230 +1742,118 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1979,89 +1972,41 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2070,23 +2015,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B95A8CAD8C29554F9E0351C467B0D6FD" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="1b39f6b3157a2808afb706e2abc1a757">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xmlns:ns4="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b35085bbad307f65ab8a7111ba96ce01" ns3:_="" ns4:_="">
     <xsd:import namespace="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
@@ -2333,32 +2261,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1904384E-797A-433F-B14D-F7DBECBCF5A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
-    <ds:schemaRef ds:uri="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23A7755D-48E6-4A04-985B-2FF9CD4824DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c3a1efe5-392e-4dcc-bcda-9894c0282c1b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB8304BA-87CC-4068-8193-05A133AC1626}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2375,4 +2295,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23A7755D-48E6-4A04-985B-2FF9CD4824DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1904384E-797A-433F-B14D-F7DBECBCF5A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="c3a1efe5-392e-4dcc-bcda-9894c0282c1b"/>
+    <ds:schemaRef ds:uri="dd2bcc39-944f-4faf-a7e7-50b5c20f56c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>